<commit_message>
Cập nhật file excel database
</commit_message>
<xml_diff>
--- a/Document/Database.xlsx
+++ b/Document/Database.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="59">
   <si>
     <t xml:space="preserve">Nhân viên</t>
   </si>
@@ -58,112 +58,145 @@
     <t xml:space="preserve">Ngày sinh</t>
   </si>
   <si>
+    <t xml:space="preserve">Giới tính</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ảnh </t>
   </si>
   <si>
+    <t xml:space="preserve">Cấp độ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 : Nhân viên</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ảnh</t>
   </si>
   <si>
-    <t xml:space="preserve">Cấp độ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0 : Nhân viên</t>
+    <t xml:space="preserve">1 : Quản lí</t>
   </si>
   <si>
     <t xml:space="preserve">Token</t>
   </si>
   <si>
-    <t xml:space="preserve">1 : Quản lí</t>
-  </si>
-  <si>
     <t xml:space="preserve">Hóa đơn</t>
   </si>
   <si>
+    <t xml:space="preserve">Sản phẩm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nhóm cấu hình</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID_khách hàng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Địa chỉ người nhận</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mô tả</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tên người nhận</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cấu hình</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SĐT người nhận</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Giá</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thời gian đặt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Số lượng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID_nhóm cấu hình</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tổng tiền hóa đơn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Đã bán</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID_nhân viên </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(nhân viên đã duyệt đơn)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xuất xứ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tình trạng đơn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0: Đang chờ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ngày ra mắt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cấu hình chi tiết</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1: Đã duyệt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID_nhà sản xuất</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID_Sản phẩm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2: Bị Hủy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID_thể loại</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID_Cấu hình</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3: Đang giao </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Giá trị</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4: Đã giao</t>
+  </si>
+  <si>
     <t xml:space="preserve">Đánh giá</t>
   </si>
   <si>
-    <t xml:space="preserve">Sản phẩm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID_khách hàng</t>
-  </si>
-  <si>
     <t xml:space="preserve">ID_hóa đơn</t>
   </si>
   <si>
-    <t xml:space="preserve">Địa chỉ người nhận</t>
-  </si>
-  <si>
     <t xml:space="preserve">ID_sản phẩm</t>
   </si>
   <si>
-    <t xml:space="preserve">Mô tả</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tên người nhận</t>
-  </si>
-  <si>
     <t xml:space="preserve">Tên người đánh giá</t>
   </si>
   <si>
-    <t xml:space="preserve">SĐT người nhận</t>
+    <t xml:space="preserve">Hóa đơn chi tiết</t>
   </si>
   <si>
     <t xml:space="preserve">Nhận xét</t>
   </si>
   <si>
-    <t xml:space="preserve">Giá</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thời gian đặt</t>
-  </si>
-  <si>
     <t xml:space="preserve">Chất lượng</t>
   </si>
   <si>
     <t xml:space="preserve">Từ 1 --&gt; 5</t>
   </si>
   <si>
-    <t xml:space="preserve">ID_nhà sản xuất</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tổng tiền hóa đơn</t>
-  </si>
-  <si>
     <t xml:space="preserve">Thời gian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID_thể loại</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID_nhân viên </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(nhân viên đã duyệt đơn)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tình trạng đơn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0: Đang chờ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1: Đã duyệt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2: Bị Hủy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3: Đang giao </t>
-  </si>
-  <si>
-    <t xml:space="preserve">4: Đã giao</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hóa đơn chi tiết</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Số lượng</t>
   </si>
 </sst>
 </file>
@@ -233,7 +266,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -269,6 +302,27 @@
       <bottom style="thin"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -295,7 +349,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -340,8 +394,28 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -369,22 +443,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K1002"/>
+  <dimension ref="A1:K1003"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="topLeft" activeCell="G26" activeCellId="0" sqref="G26:G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="10" style="0" width="7.63"/>
   </cols>
@@ -516,7 +590,7 @@
       <c r="B8" s="7"/>
       <c r="C8" s="2"/>
       <c r="D8" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="10" t="s">
@@ -530,15 +604,15 @@
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="2"/>
       <c r="D9" s="9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="F9" s="11"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -553,7 +627,7 @@
         <v>15</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E10" s="2"/>
@@ -565,12 +639,13 @@
       <c r="K10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="12" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="D11" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -580,8 +655,8 @@
       <c r="K11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="14"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -593,37 +668,29 @@
       <c r="K12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="4"/>
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
       <c r="C13" s="2"/>
-      <c r="D13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="4"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="9"/>
+      <c r="A14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="4"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="E14" s="9"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="9" t="s">
-        <v>3</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -632,17 +699,15 @@
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="9" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="2"/>
       <c r="D15" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="9"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="9" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>3</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -651,17 +716,15 @@
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" s="9"/>
       <c r="C16" s="2"/>
       <c r="D16" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="9" t="s">
-        <v>25</v>
+        <v>5</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>5</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -670,18 +733,14 @@
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="2"/>
       <c r="D17" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="9"/>
+        <v>24</v>
+      </c>
       <c r="F17" s="2"/>
-      <c r="G17" s="9" t="s">
-        <v>13</v>
-      </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -689,17 +748,15 @@
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B18" s="9"/>
       <c r="C18" s="2"/>
       <c r="D18" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E18" s="9"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="9" t="s">
-        <v>30</v>
+        <v>16</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
@@ -708,19 +765,15 @@
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B19" s="9"/>
       <c r="C19" s="2"/>
       <c r="D19" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="9" t="s">
-        <v>34</v>
+        <v>28</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>3</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -729,17 +782,15 @@
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="9" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B20" s="9"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E20" s="10"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="10" t="s">
-        <v>37</v>
+      <c r="D20" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>31</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -748,16 +799,16 @@
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>39</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="B21" s="9"/>
       <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
+      <c r="D21" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>5</v>
+      </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -765,31 +816,37 @@
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
+      <c r="D22" s="15" t="s">
+        <v>36</v>
+      </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="6"/>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="9"/>
-      <c r="B23" s="12" t="s">
-        <v>42</v>
+      <c r="A23" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
+      <c r="D23" s="15" t="s">
+        <v>39</v>
+      </c>
       <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
+      <c r="F23" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
@@ -797,14 +854,17 @@
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="9"/>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -812,45 +872,45 @@
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="9"/>
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="17" t="s">
         <v>44</v>
       </c>
       <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
+      <c r="D25" s="16" t="s">
+        <v>45</v>
+      </c>
       <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
+      <c r="F25" s="15" t="s">
+        <v>46</v>
+      </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="6"/>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="10"/>
-      <c r="B26" s="13" t="s">
-        <v>45</v>
+      <c r="A26" s="9"/>
+      <c r="B26" s="17" t="s">
+        <v>47</v>
       </c>
       <c r="C26" s="2"/>
-      <c r="D26" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="D26" s="2"/>
       <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
+      <c r="F26" s="16" t="s">
+        <v>48</v>
+      </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="6"/>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
+      <c r="A27" s="10"/>
+      <c r="B27" s="18" t="s">
+        <v>49</v>
+      </c>
       <c r="C27" s="2"/>
-      <c r="D27" s="9" t="s">
-        <v>22</v>
-      </c>
       <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
@@ -861,11 +921,7 @@
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="9" t="s">
-        <v>24</v>
-      </c>
       <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
@@ -876,11 +932,7 @@
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="10" t="s">
-        <v>47</v>
-      </c>
       <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
@@ -888,11 +940,12 @@
       <c r="K29" s="6"/>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2"/>
+      <c r="A30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" s="4"/>
       <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
       <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
@@ -900,11 +953,13 @@
       <c r="K30" s="6"/>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2"/>
+      <c r="A31" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" s="9"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
@@ -912,11 +967,13 @@
       <c r="K31" s="6"/>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="2"/>
+      <c r="A32" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" s="9"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
@@ -924,11 +981,13 @@
       <c r="K32" s="6"/>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="2"/>
+      <c r="A33" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" s="9"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
@@ -936,12 +995,15 @@
       <c r="K33" s="6"/>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
+      <c r="A34" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" s="9"/>
       <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
+      <c r="D34" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
@@ -949,12 +1011,15 @@
       <c r="K34" s="6"/>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
+      <c r="A35" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" s="9"/>
       <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
+      <c r="D35" s="9" t="s">
+        <v>51</v>
+      </c>
       <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
@@ -962,25 +1027,33 @@
       <c r="K35" s="6"/>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="6"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
+      <c r="A36" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" s="2"/>
+      <c r="D36" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
       <c r="K36" s="6"/>
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
+      <c r="A37" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B37" s="10"/>
       <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
+      <c r="D37" s="10" t="s">
+        <v>30</v>
+      </c>
       <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
       <c r="G37" s="6"/>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
@@ -993,7 +1066,6 @@
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
       <c r="G38" s="6"/>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
@@ -1338,7 +1410,19 @@
       <c r="J64" s="6"/>
       <c r="K64" s="6"/>
     </row>
-    <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A65" s="6"/>
+      <c r="B65" s="6"/>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="6"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="6"/>
+      <c r="H65" s="6"/>
+      <c r="I65" s="6"/>
+      <c r="J65" s="6"/>
+      <c r="K65" s="6"/>
+    </row>
     <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="67" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="68" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2276,11 +2360,12 @@
     <row r="1000" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1001" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1002" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1003" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A30:B30"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Cập nhật gio hang va don mua
</commit_message>
<xml_diff>
--- a/Document/Database.xlsx
+++ b/Document/Database.xlsx
@@ -136,7 +136,7 @@
     <t xml:space="preserve">Tình trạng đơn</t>
   </si>
   <si>
-    <t xml:space="preserve">0: Đang chờ </t>
+    <t xml:space="preserve">0: Bị Hủy</t>
   </si>
   <si>
     <t xml:space="preserve">Ngày ra mắt</t>
@@ -145,7 +145,7 @@
     <t xml:space="preserve">Cấu hình chi tiết</t>
   </si>
   <si>
-    <t xml:space="preserve">1: Đã duyệt</t>
+    <t xml:space="preserve">1: Đang chờ</t>
   </si>
   <si>
     <t xml:space="preserve">ID_nhà sản xuất</t>
@@ -154,7 +154,7 @@
     <t xml:space="preserve">ID_Sản phẩm</t>
   </si>
   <si>
-    <t xml:space="preserve">2: Bị Hủy</t>
+    <t xml:space="preserve">2: Đã duyệt</t>
   </si>
   <si>
     <t xml:space="preserve">ID_thể loại</t>
@@ -617,11 +617,11 @@
   </sheetPr>
   <dimension ref="A1:K1003"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F48" activeCellId="0" sqref="F48"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.59375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.38"/>
@@ -1008,7 +1008,7 @@
       <c r="A23" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="17" t="s">
         <v>38</v>
       </c>
       <c r="C23" s="2"/>

</xml_diff>